<commit_message>
reports for all country + fixed codes in Rmd
</commit_message>
<xml_diff>
--- a/Comments on each country.xlsx
+++ b/Comments on each country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktang3\Desktop\Imperial\Pop_Construct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0DCE365-098E-4C0C-903E-8750D34DCC21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A6E7FC-135D-4F0A-8DC7-20E93C5D3C2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{4BCE925D-0329-41F2-AB77-93E1313221D2}"/>
   </bookViews>
@@ -34,20 +34,254 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Angola</t>
   </si>
   <si>
     <t>Only 1 census (in2014) from DYB after 1960 (also one in 1960 but atm using WPP 1960 for generality)</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cesus period labelling </t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>CDR</t>
+  </si>
+  <si>
+    <t>only 1 census (in 1955) from DYB + DDHarmony error</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Estimated Epsilon too high?</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Male estimated B wiggly, female lambda &gt; male lambda, female mort &gt; male mort at 10-14 and 15-19 in early years</t>
+  </si>
+  <si>
+    <t>Male lambda vs female lambda shape, and female lambda &gt; male lambda</t>
+  </si>
+  <si>
+    <t>Consistent lower estimates compared to the WPP/IGME U5MR, over-smoothed hump at early years? (try reverse RW), female lambda &gt; male lambda</t>
+  </si>
+  <si>
+    <t>Unrealisetic AB term, cross over of 45q15, over-smoothed hump from DHS? Female lambda &gt; male lambda</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Restricted Data failed to converge, female lambda &gt; male lambda, something happened in 1995, migration proportion wiggly</t>
+  </si>
+  <si>
+    <t>Eswatini</t>
+  </si>
+  <si>
+    <t>Estimated Epsilon too high? Unrealistic migration?</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Female lambda &gt; male lambda and wiggly, cross over 45q15 in early years, over-smoothed humps from DHS?</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Messy estimated B, spike in 45q15 in 1975, estimated mort schedules using full data vs restricted differ a lot (coz of B)!</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Cross over 45q15 at the earliest years</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Unrealistic female A, female lambda &gt; male lambda, cross over 45q15 in early years, male U5MR lower than WPP/IGME estimates in all years, over-smoothed humps? Kink in mort schedules over time at older ages in 1995</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>female lambda &gt; male lambda, unrealistic psi and AB term (coz of the spike in 1985 also seen in GBD estimates?), lower male U5MR than WPP/IGME. Need to double check spline estimates whether wiggly over time</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>female lambda &gt; male lambda at the most recent years, questionable female A? Cross over 45q15 early years, over-smoothed humps? Unrealistic migration</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Restricted Data failed to converge, female lambda &gt; male lambda, wiggly psi, female A &gt; male A, cross over 45q15 in early years, over-smoothed humps?</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>female lambda &gt; male lambda, cross over 45q15 in early years, questionable migration?</t>
+  </si>
+  <si>
+    <t>Requires different initial values (init marginal_prec = 2, rho = 2), whole thing is wrong, need to experiment without DHS and see! Female lambda &gt; male lambda when using full data, unrealistic AB term when using full data, unrealistic migration</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Requires different prior means for the hump componenet to converge (lambda = 0.008, delta = 1), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wouldn’t converge with restricted data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, unrealistic AB term, female mort schedule too sharp at 15?</t>
+    </r>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Requires different prior means for the hump componenet to converge (lambda = 0.003, delta = 0.2, i.e. hard-coded a flat hump), wouldn’t converge with restricted data. These priors mean a very flat hump, otherwise extreme values for epsilon are returned, possibly due to the very flat mort schedule seen in DHS data.</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Requires different initial values (init hump.marginal_prec = 0, rho = 0), female lambda &gt; male lambda (but possible?), unrealistic female A &gt; male A,.</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Requires different initial values (init hump.marginal_prec=0, rho=2, marginal_prec = 4), unrealistic AB term, epsilon too high? WPP U5MR estimates also seem unrealistic?</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Requires diff initial values (init hump.marginal.prec = 2, rho=0, marginal.prec=3), female U5MR lower than WPP/IGME</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Requires diff initial values (init hump.marginal.prec = 2, rho=0, marginal.prec=3), failed to converged with restricted data, messy results, double check with spline estimates, wiggly over time as well?</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Migration is wonky, deviation from initial fert estimates are large, 45q15 consistently lower than GBD/WPP</t>
+  </si>
+  <si>
+    <t>female A &gt; male A, female AB term wiggly, female 45q15 earliest years questionable</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wouldn't converge with restricted data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, female A &gt; male A</t>
+    </r>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Female A &gt; male A</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Requires different prior means for the hump componenet to converge (lambda = 0.003, delta = 0.3, i.e. hard-coded a flat hump), female lambda &gt; male lambda, wiggly AB term</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>AB term, restricted data failes to converge</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -391,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4106BF-524D-44FF-944F-761B2564C984}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,7 +644,253 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RW with tight AB and LQ initial prior + RW and A diff term
</commit_message>
<xml_diff>
--- a/Comments on each country.xlsx
+++ b/Comments on each country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktang3\Desktop\Imperial\Pop_Construct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A6E7FC-135D-4F0A-8DC7-20E93C5D3C2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B29F915-3E70-4A71-96EC-48A594A170FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{4BCE925D-0329-41F2-AB77-93E1313221D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Angola</t>
   </si>
@@ -153,8 +153,94 @@
     <t>Lesotho</t>
   </si>
   <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Requires different prior means for the hump componenet to converge (lambda = 0.003, delta = 0.2, i.e. hard-coded a flat hump), wouldn’t converge with restricted data. These priors mean a very flat hump, otherwise extreme values for epsilon are returned, possibly due to the very flat mort schedule seen in DHS data.</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Requires different initial values (init hump.marginal_prec=0, rho=2, marginal_prec = 4), unrealistic AB term, epsilon too high? WPP U5MR estimates also seem unrealistic?</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Requires diff initial values (init hump.marginal.prec = 2, rho=0, marginal.prec=3), female U5MR lower than WPP/IGME</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Requires diff initial values (init hump.marginal.prec = 2, rho=0, marginal.prec=3), failed to converged with restricted data, messy results, double check with spline estimates, wiggly over time as well?</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Migration is wonky, deviation from initial fert estimates are large, 45q15 consistently lower than GBD/WPP</t>
+  </si>
+  <si>
+    <t>female A &gt; male A, female AB term wiggly, female 45q15 earliest years questionable</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Requires different prior means for the hump componenet to converge (lambda = 0.008, delta = 1), </t>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wouldn't converge with restricted data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, female A &gt; male A</t>
+    </r>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Female A &gt; male A</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Requires different prior means for the hump componenet to converge (lambda = 0.003, delta = 0.3, i.e. hard-coded a flat hump), female lambda &gt; male lambda, wiggly AB term</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>AB term, restricted data failes to converge</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Requires different prior means for the hump component to converge (lambda = 0.008, delta = 1), </t>
     </r>
     <r>
       <rPr>
@@ -179,93 +265,10 @@
     </r>
   </si>
   <si>
-    <t>Madagascar</t>
-  </si>
-  <si>
-    <t>Requires different prior means for the hump componenet to converge (lambda = 0.003, delta = 0.2, i.e. hard-coded a flat hump), wouldn’t converge with restricted data. These priors mean a very flat hump, otherwise extreme values for epsilon are returned, possibly due to the very flat mort schedule seen in DHS data.</t>
-  </si>
-  <si>
-    <t>Malawi</t>
-  </si>
-  <si>
-    <t>Requires different initial values (init hump.marginal_prec = 0, rho = 0), female lambda &gt; male lambda (but possible?), unrealistic female A &gt; male A,.</t>
-  </si>
-  <si>
-    <t>Namibia</t>
-  </si>
-  <si>
-    <t>Rwanda</t>
-  </si>
-  <si>
-    <t>Requires different initial values (init hump.marginal_prec=0, rho=2, marginal_prec = 4), unrealistic AB term, epsilon too high? WPP U5MR estimates also seem unrealistic?</t>
-  </si>
-  <si>
-    <t>Senegal</t>
-  </si>
-  <si>
-    <t>Requires diff initial values (init hump.marginal.prec = 2, rho=0, marginal.prec=3), female U5MR lower than WPP/IGME</t>
-  </si>
-  <si>
-    <t>Sierra Leone</t>
-  </si>
-  <si>
-    <t>Requires diff initial values (init hump.marginal.prec = 2, rho=0, marginal.prec=3), failed to converged with restricted data, messy results, double check with spline estimates, wiggly over time as well?</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Zambia</t>
-  </si>
-  <si>
-    <t>Migration is wonky, deviation from initial fert estimates are large, 45q15 consistently lower than GBD/WPP</t>
-  </si>
-  <si>
-    <t>female A &gt; male A, female AB term wiggly, female 45q15 earliest years questionable</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Wouldn't converge with restricted data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, female A &gt; male A</t>
-    </r>
-  </si>
-  <si>
-    <t>Tanzania</t>
-  </si>
-  <si>
-    <t>Female A &gt; male A</t>
-  </si>
-  <si>
-    <t>Togo</t>
-  </si>
-  <si>
-    <t>Requires different prior means for the hump componenet to converge (lambda = 0.003, delta = 0.3, i.e. hard-coded a flat hump), female lambda &gt; male lambda, wiggly AB term</t>
-  </si>
-  <si>
-    <t>Uganda</t>
-  </si>
-  <si>
-    <t>AB term, restricted data failes to converge</t>
-  </si>
-  <si>
-    <t>Zimbabwe</t>
+    <t>Requires different initial values (init hump.marginal_prec = 0, rho = 0), female lambda &gt; male lambda (but possible?), unrealistic female A &gt; male A</t>
+  </si>
+  <si>
+    <t>delta</t>
   </si>
 </sst>
 </file>
@@ -625,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4106BF-524D-44FF-944F-761B2564C984}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,7 +756,7 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -764,23 +767,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -788,7 +791,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -796,15 +799,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -812,7 +815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -820,73 +823,76 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>60</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>